<commit_message>
Updated Marks Contribution Spreadsheet
</commit_message>
<xml_diff>
--- a/SEMspreadsheet.xlsx
+++ b/SEMspreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\School of Computing\User Data\40541783\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E40B63D-0108-487B-9B3F-0740587FFD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD72AD8-A7FE-4A9C-A55D-499479BA7C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -105,6 +105,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +426,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,20 +460,32 @@
       <c r="A2" s="2">
         <v>40536446</v>
       </c>
+      <c r="B2" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>40125848</v>
       </c>
+      <c r="B3" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40541783</v>
       </c>
+      <c r="B4" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40618094</v>
+      </c>
+      <c r="B5" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Add queries from 1 to 22
</commit_message>
<xml_diff>
--- a/SEMspreadsheet.xlsx
+++ b/SEMspreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\School of Computing\User Data\40541783\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\java\seMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD72AD8-A7FE-4A9C-A55D-499479BA7C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB77E6F-5EB3-4B65-80DB-A21AA131681B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +463,12 @@
       <c r="B2" s="4">
         <v>25</v>
       </c>
+      <c r="C2" s="4">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -471,6 +477,12 @@
       <c r="B3" s="4">
         <v>25</v>
       </c>
+      <c r="C3" s="4">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -479,12 +491,24 @@
       <c r="B4" s="4">
         <v>25</v>
       </c>
+      <c r="C4" s="4">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40618094</v>
       </c>
       <c r="B5" s="4">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4">
         <v>25</v>
       </c>
     </row>

</xml_diff>